<commit_message>
fix: update data dictionnary.
</commit_message>
<xml_diff>
--- a/Dictionnaire De Donne .xlsx
+++ b/Dictionnaire De Donne .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="86">
   <si>
     <t>ENTITY</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">password of the user </t>
   </si>
   <si>
-    <t>******</t>
+    <t>password123</t>
   </si>
   <si>
     <t>BOOK</t>
@@ -160,7 +160,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>DD/MM/YYYY</t>
+    <t>YYYY/MM/DD</t>
   </si>
   <si>
     <t>number_of_copies</t>
@@ -220,25 +220,16 @@
     <t>date of the loan</t>
   </si>
   <si>
-    <t>21/06/2024</t>
-  </si>
-  <si>
-    <t>excepted_return_date</t>
+    <t>excpected_return_date</t>
   </si>
   <si>
     <t>excepected return date</t>
   </si>
   <si>
-    <t>21/07/2024</t>
-  </si>
-  <si>
     <t>actual_return_date</t>
   </si>
   <si>
     <t>actual return date</t>
-  </si>
-  <si>
-    <t>25/07/2024</t>
   </si>
   <si>
     <t>RESERVATION</t>
@@ -284,8 +275,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -372,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -411,6 +403,9 @@
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -835,7 +830,7 @@
         <v>14</v>
       </c>
       <c r="E11" s="3">
-        <v>6.0</v>
+        <v>50.0</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>33</v>
@@ -967,7 +962,7 @@
         <v>49</v>
       </c>
       <c r="G19" s="10">
-        <v>38477.0</v>
+        <v>45041.0</v>
       </c>
     </row>
     <row r="20">
@@ -1167,17 +1162,17 @@
       <c r="F30" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>69</v>
+      <c r="G30" s="17">
+        <v>45464.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="15"/>
       <c r="B31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>48</v>
@@ -1188,17 +1183,17 @@
       <c r="F31" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>72</v>
+      <c r="G31" s="17">
+        <v>45494.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="15"/>
       <c r="B32" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>48</v>
@@ -1209,8 +1204,8 @@
       <c r="F32" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>75</v>
+      <c r="G32" s="17">
+        <v>45498.0</v>
       </c>
     </row>
     <row r="33">
@@ -1242,8 +1237,8 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34">
-      <c r="A34" s="17" t="s">
-        <v>76</v>
+      <c r="A34" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -1272,12 +1267,12 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35">
-      <c r="A35" s="18"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>10</v>
@@ -1293,12 +1288,12 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="18"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>48</v>
@@ -1309,13 +1304,13 @@
       <c r="F36" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>69</v>
+      <c r="G36" s="17">
+        <v>45464.0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="19" t="s">
-        <v>81</v>
+      <c r="A38" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -1344,12 +1339,12 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39">
-      <c r="A39" s="20"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>10</v>
@@ -1365,12 +1360,12 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="20"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>48</v>
@@ -1381,17 +1376,17 @@
       <c r="F40" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>75</v>
+      <c r="G40" s="17">
+        <v>45546.0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="20"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>14</v>
@@ -1400,7 +1395,7 @@
         <v>50.0</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43">

</xml_diff>